<commit_message>
Lots of work sorting out data munging and calls to the Zillow API
</commit_message>
<xml_diff>
--- a/inputs/desaster_input_data_template.xlsx
+++ b/inputs/desaster_input_data_template.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28810"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10311"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/geomando/Dropbox/github/DESaster/inputs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/geomando/Dropbox/github/NapaCountyDESaster/inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F15D5511-3BCA-8444-A913-DCF679C074F0}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="80" yWindow="460" windowWidth="28720" windowHeight="17540" tabRatio="500"/>
+    <workbookView xWindow="80" yWindow="460" windowWidth="28720" windowHeight="17540" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="renters" sheetId="5" r:id="rId1"/>
@@ -18,7 +19,7 @@
     <sheet name="forrent_stock" sheetId="6" r:id="rId4"/>
     <sheet name="temp_stock" sheetId="7" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -282,8 +283,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1517,6 +1518,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -1783,19 +1787,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="16" max="16" width="16.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:23">
       <c r="A1" t="s">
         <v>81</v>
       </c>
@@ -1866,7 +1870,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:23">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -1941,7 +1945,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:23">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -2016,7 +2020,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:23">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -2090,7 +2094,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="5" spans="1:23" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:23" s="4" customFormat="1">
       <c r="A5" s="4" t="s">
         <v>18</v>
       </c>
@@ -2165,7 +2169,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:23">
       <c r="A6" t="s">
         <v>35</v>
       </c>
@@ -2239,7 +2243,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:23">
       <c r="A7" t="s">
         <v>36</v>
       </c>
@@ -2313,7 +2317,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:23">
       <c r="A8" t="s">
         <v>38</v>
       </c>
@@ -2387,7 +2391,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="9" spans="1:23" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:23" s="4" customFormat="1">
       <c r="A9" s="4" t="s">
         <v>39</v>
       </c>
@@ -2468,19 +2472,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:S10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="P2" sqref="P2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="16" max="16" width="16.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19" s="4" customFormat="1">
       <c r="A1" s="4" t="s">
         <v>71</v>
       </c>
@@ -2539,7 +2543,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="2" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:19" s="4" customFormat="1">
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
@@ -2601,7 +2605,7 @@
         <v>43.224344000000002</v>
       </c>
     </row>
-    <row r="3" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:19" s="4" customFormat="1">
       <c r="A3" s="4" t="s">
         <v>3</v>
       </c>
@@ -2663,7 +2667,7 @@
         <v>43.224218999999998</v>
       </c>
     </row>
-    <row r="4" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:19" s="4" customFormat="1">
       <c r="A4" s="4" t="s">
         <v>6</v>
       </c>
@@ -2725,7 +2729,7 @@
         <v>43.223984000000002</v>
       </c>
     </row>
-    <row r="5" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:19" s="4" customFormat="1">
       <c r="A5" s="4" t="s">
         <v>9</v>
       </c>
@@ -2787,7 +2791,7 @@
         <v>43.223750000000003</v>
       </c>
     </row>
-    <row r="6" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:19" s="4" customFormat="1">
       <c r="A6" s="4" t="s">
         <v>32</v>
       </c>
@@ -2848,7 +2852,7 @@
         <v>43.224375000000002</v>
       </c>
     </row>
-    <row r="7" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:19" s="4" customFormat="1">
       <c r="A7" s="4" t="s">
         <v>33</v>
       </c>
@@ -2909,7 +2913,7 @@
         <v>43.224390999999997</v>
       </c>
     </row>
-    <row r="8" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:19" s="4" customFormat="1">
       <c r="A8" s="4" t="s">
         <v>37</v>
       </c>
@@ -2971,7 +2975,7 @@
         <v>43.223953000000002</v>
       </c>
     </row>
-    <row r="9" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:19" s="4" customFormat="1">
       <c r="A9" s="4" t="s">
         <v>34</v>
       </c>
@@ -3032,7 +3036,7 @@
         <v>43.223717999999998</v>
       </c>
     </row>
-    <row r="10" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="10" spans="1:19" s="4" customFormat="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -3040,16 +3044,16 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:S10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J29" sqref="J29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
-    <row r="1" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19" s="4" customFormat="1">
       <c r="A1" s="4" t="s">
         <v>58</v>
       </c>
@@ -3108,7 +3112,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="2" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:19" s="4" customFormat="1">
       <c r="A2" s="4" t="s">
         <v>11</v>
       </c>
@@ -3169,7 +3173,7 @@
         <v>850</v>
       </c>
     </row>
-    <row r="3" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:19" s="4" customFormat="1">
       <c r="A3" s="4" t="s">
         <v>12</v>
       </c>
@@ -3230,7 +3234,7 @@
         <v>850</v>
       </c>
     </row>
-    <row r="4" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:19" s="4" customFormat="1">
       <c r="A4" s="4" t="s">
         <v>13</v>
       </c>
@@ -3292,7 +3296,7 @@
         <v>850</v>
       </c>
     </row>
-    <row r="5" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:19" s="4" customFormat="1">
       <c r="A5" s="4" t="s">
         <v>14</v>
       </c>
@@ -3353,7 +3357,7 @@
         <v>850</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:19">
       <c r="O10" s="4"/>
       <c r="P10" s="4"/>
       <c r="Q10" s="4"/>
@@ -3367,20 +3371,20 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:R11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="5" max="5" width="16.83203125" customWidth="1"/>
     <col min="10" max="10" width="12.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:18">
       <c r="A1" s="2" t="s">
         <v>58</v>
       </c>
@@ -3436,7 +3440,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:18">
       <c r="A2" t="s">
         <v>23</v>
       </c>
@@ -3495,7 +3499,7 @@
         <v>850</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:18">
       <c r="A3" t="s">
         <v>24</v>
       </c>
@@ -3554,7 +3558,7 @@
         <v>850</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:18">
       <c r="A4" t="s">
         <v>25</v>
       </c>
@@ -3613,7 +3617,7 @@
         <v>850</v>
       </c>
     </row>
-    <row r="5" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:18" s="4" customFormat="1">
       <c r="A5" s="4" t="s">
         <v>26</v>
       </c>
@@ -3672,7 +3676,7 @@
         <v>850</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:18">
       <c r="A6" t="s">
         <v>47</v>
       </c>
@@ -3729,7 +3733,7 @@
         <v>850</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:18">
       <c r="A7" s="2" t="s">
         <v>48</v>
       </c>
@@ -3786,7 +3790,7 @@
         <v>850</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:18">
       <c r="A8" t="s">
         <v>50</v>
       </c>
@@ -3842,7 +3846,7 @@
         <v>850</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:18">
       <c r="A9" t="s">
         <v>55</v>
       </c>
@@ -3898,7 +3902,7 @@
         <v>850</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:18">
       <c r="A10" t="s">
         <v>56</v>
       </c>
@@ -3954,7 +3958,7 @@
         <v>850</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:18">
       <c r="A11" t="s">
         <v>57</v>
       </c>
@@ -4017,19 +4021,19 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:R11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="11" max="11" width="16.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:18">
       <c r="A1" s="2" t="s">
         <v>58</v>
       </c>
@@ -4085,7 +4089,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:18">
       <c r="A2" s="2" t="s">
         <v>23</v>
       </c>
@@ -4141,7 +4145,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:18">
       <c r="A3" s="2" t="s">
         <v>24</v>
       </c>
@@ -4197,7 +4201,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:18">
       <c r="A4" s="2" t="s">
         <v>25</v>
       </c>
@@ -4253,7 +4257,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:18">
       <c r="A5" s="2" t="s">
         <v>26</v>
       </c>
@@ -4309,7 +4313,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:18">
       <c r="A6" s="2" t="s">
         <v>47</v>
       </c>
@@ -4365,7 +4369,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:18">
       <c r="A7" s="2" t="s">
         <v>48</v>
       </c>
@@ -4421,7 +4425,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:18">
       <c r="A8" s="2" t="s">
         <v>50</v>
       </c>
@@ -4477,7 +4481,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:18">
       <c r="A9" s="2" t="s">
         <v>55</v>
       </c>
@@ -4533,7 +4537,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:18">
       <c r="A10" s="2" t="s">
         <v>56</v>
       </c>
@@ -4589,7 +4593,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:18">
       <c r="A11" s="2" t="s">
         <v>57</v>
       </c>

</xml_diff>